<commit_message>
added new data file for all and script for supplementary plots
</commit_message>
<xml_diff>
--- a/DATA/R3_data.xlsx
+++ b/DATA/R3_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauraelsler/Dropbox/PhD/Resources/P2/Squid/Laura/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauraelsler/Dropbox/PhD/Resources/SQUID/Squid/CODE/Squid/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8BCDDD31-2529-C145-9C76-D2A3DDF58910}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB308431-7385-6F4B-B107-1C219C186FD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8800" yWindow="460" windowWidth="16800" windowHeight="14260" xr2:uid="{FC4F04E1-F260-514A-A0DB-5179CCD70447}"/>
+    <workbookView xWindow="8800" yWindow="460" windowWidth="16800" windowHeight="14100" xr2:uid="{FC4F04E1-F260-514A-A0DB-5179CCD70447}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>year</t>
   </si>
@@ -50,69 +50,6 @@
   </si>
   <si>
     <t>y_S</t>
-  </si>
-  <si>
-    <t>0.0684643305769838</t>
-  </si>
-  <si>
-    <t>0.403634978261844</t>
-  </si>
-  <si>
-    <t>0.000654912707029971</t>
-  </si>
-  <si>
-    <t>0.101077368850753</t>
-  </si>
-  <si>
-    <t>0.0298536072366519</t>
-  </si>
-  <si>
-    <t>0.0462491949003793</t>
-  </si>
-  <si>
-    <t>0.0195848927351414</t>
-  </si>
-  <si>
-    <t>0.045536408800866</t>
-  </si>
-  <si>
-    <t>0.116473106537236</t>
-  </si>
-  <si>
-    <t>0.0547643279285915</t>
-  </si>
-  <si>
-    <t>0.0783847880446964</t>
-  </si>
-  <si>
-    <t>0.0868640510498765</t>
-  </si>
-  <si>
-    <t>0.0956260552611002</t>
-  </si>
-  <si>
-    <t>0.442268155099306</t>
-  </si>
-  <si>
-    <t>0.343883223114352</t>
-  </si>
-  <si>
-    <t>0.402384408016426</t>
-  </si>
-  <si>
-    <t>0.630465863494975</t>
-  </si>
-  <si>
-    <t>0.135463067697345</t>
-  </si>
-  <si>
-    <t>0.538182595934376</t>
-  </si>
-  <si>
-    <t>0.403669935043269</t>
-  </si>
-  <si>
-    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -472,10 +409,18 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -513,7 +458,7 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -530,7 +475,7 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>1</v>
       </c>
     </row>
@@ -547,7 +492,7 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>1</v>
       </c>
     </row>
@@ -567,7 +512,7 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1</v>
       </c>
     </row>
@@ -587,7 +532,7 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>1</v>
       </c>
     </row>
@@ -607,7 +552,7 @@
       <c r="F7" s="1">
         <v>60.2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>1</v>
       </c>
     </row>
@@ -627,8 +572,8 @@
       <c r="F8" s="1">
         <v>68.7</v>
       </c>
-      <c r="G8" t="s">
-        <v>7</v>
+      <c r="G8" s="1">
+        <v>6.8464330576983798E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -647,8 +592,8 @@
       <c r="F9" s="1">
         <v>28.7</v>
       </c>
-      <c r="G9" t="s">
-        <v>8</v>
+      <c r="G9" s="1">
+        <v>0.40363497826184402</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -667,8 +612,8 @@
       <c r="F10" s="1">
         <v>46.8</v>
       </c>
-      <c r="G10" t="s">
-        <v>9</v>
+      <c r="G10" s="1">
+        <v>6.5491270702997104E-4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -687,8 +632,8 @@
       <c r="F11" s="1">
         <v>35.799999999999997</v>
       </c>
-      <c r="G11" t="s">
-        <v>10</v>
+      <c r="G11" s="1">
+        <v>0.101077368850753</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -710,8 +655,8 @@
       <c r="F12" s="1">
         <v>50.4</v>
       </c>
-      <c r="G12" t="s">
-        <v>11</v>
+      <c r="G12" s="1">
+        <v>2.98536072366519E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -733,8 +678,8 @@
       <c r="F13" s="1">
         <v>65.599999999999994</v>
       </c>
-      <c r="G13" t="s">
-        <v>12</v>
+      <c r="G13" s="1">
+        <v>4.6249194900379299E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -756,8 +701,8 @@
       <c r="F14" s="1">
         <v>56.4</v>
       </c>
-      <c r="G14" t="s">
-        <v>13</v>
+      <c r="G14" s="1">
+        <v>1.9584892735141399E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -779,8 +724,8 @@
       <c r="F15" s="1">
         <v>64.8</v>
       </c>
-      <c r="G15" t="s">
-        <v>14</v>
+      <c r="G15" s="1">
+        <v>4.5536408800865999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -802,8 +747,8 @@
       <c r="F16" s="1">
         <v>59.6</v>
       </c>
-      <c r="G16" t="s">
-        <v>15</v>
+      <c r="G16" s="1">
+        <v>0.116473106537236</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -825,8 +770,8 @@
       <c r="F17" s="1">
         <v>62.9</v>
       </c>
-      <c r="G17" t="s">
-        <v>16</v>
+      <c r="G17" s="1">
+        <v>5.4764327928591497E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -848,8 +793,8 @@
       <c r="F18" s="1">
         <v>66.7</v>
       </c>
-      <c r="G18" t="s">
-        <v>17</v>
+      <c r="G18" s="1">
+        <v>7.8384788044696396E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -871,8 +816,8 @@
       <c r="F19" s="1">
         <v>69.2</v>
       </c>
-      <c r="G19" t="s">
-        <v>18</v>
+      <c r="G19" s="1">
+        <v>8.6864051049876503E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -894,8 +839,8 @@
       <c r="F20" s="1">
         <v>30.8</v>
       </c>
-      <c r="G20" t="s">
-        <v>19</v>
+      <c r="G20" s="1">
+        <v>9.5626055261100198E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -917,8 +862,8 @@
       <c r="F21" s="1">
         <v>46</v>
       </c>
-      <c r="G21" t="s">
-        <v>20</v>
+      <c r="G21" s="1">
+        <v>0.442268155099306</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -940,8 +885,8 @@
       <c r="F22" s="1">
         <v>32.5</v>
       </c>
-      <c r="G22" t="s">
-        <v>21</v>
+      <c r="G22" s="1">
+        <v>0.34388322311435199</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -960,8 +905,8 @@
       <c r="F23" s="1">
         <v>36.4</v>
       </c>
-      <c r="G23" t="s">
-        <v>22</v>
+      <c r="G23" s="1">
+        <v>0.402384408016426</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -980,8 +925,8 @@
       <c r="F24" s="1">
         <v>45</v>
       </c>
-      <c r="G24" t="s">
-        <v>23</v>
+      <c r="G24" s="1">
+        <v>0.63046586349497502</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1000,8 +945,8 @@
       <c r="F25" s="1">
         <v>46.1</v>
       </c>
-      <c r="G25" t="s">
-        <v>24</v>
+      <c r="G25" s="1">
+        <v>0.13546306769734501</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1023,8 +968,8 @@
       <c r="F26" s="1">
         <v>20.100000000000001</v>
       </c>
-      <c r="G26" t="s">
-        <v>25</v>
+      <c r="G26" s="1">
+        <v>0.53818259593437601</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1046,8 +991,8 @@
       <c r="F27" s="1">
         <v>18.100000000000001</v>
       </c>
-      <c r="G27" t="s">
-        <v>26</v>
+      <c r="G27" s="1">
+        <v>0.40366993504326898</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1057,8 +1002,8 @@
       <c r="F28" s="1">
         <v>21.4</v>
       </c>
-      <c r="G28" t="s">
-        <v>27</v>
+      <c r="G28" s="1">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>